<commit_message>
results!!! also removed df.head(50) and k1=k2=5
</commit_message>
<xml_diff>
--- a/project2Table1.xlsx
+++ b/project2Table1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,19 +465,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>2409.982969171706</v>
+        <v>458.8499701346049</v>
       </c>
       <c r="D2" t="n">
         <v>1500</v>
       </c>
       <c r="E2" t="n">
-        <v>501.4169176609875</v>
+        <v>457.524951905785</v>
       </c>
       <c r="F2" t="n">
-        <v>872.5961809942004</v>
+        <v>809.2470893547023</v>
       </c>
     </row>
     <row r="3">
@@ -485,19 +485,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>4574.189288021799</v>
+        <v>566.9923819505786</v>
       </c>
       <c r="D3" t="n">
         <v>1500</v>
       </c>
       <c r="E3" t="n">
-        <v>481.7493993398917</v>
+        <v>544.4008421964322</v>
       </c>
       <c r="F3" t="n">
-        <v>916.8971578536606</v>
+        <v>935.9457710565886</v>
       </c>
     </row>
     <row r="4">
@@ -505,19 +505,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>3236.436379425283</v>
+        <v>3897.301207536528</v>
       </c>
       <c r="D4" t="n">
         <v>1500</v>
       </c>
       <c r="E4" t="n">
-        <v>497.8493145848994</v>
+        <v>421.3954489148648</v>
       </c>
       <c r="F4" t="n">
-        <v>918.4511492898976</v>
+        <v>822.6894271705743</v>
       </c>
     </row>
     <row r="5">
@@ -525,19 +525,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>512.2958231264255</v>
+        <v>583.1179766099127</v>
       </c>
       <c r="D5" t="n">
         <v>1500</v>
       </c>
       <c r="E5" t="n">
-        <v>507.6553607072717</v>
+        <v>541.0500768672667</v>
       </c>
       <c r="F5" t="n">
-        <v>916.3877269873985</v>
+        <v>1010.930492410078</v>
       </c>
     </row>
     <row r="6">
@@ -545,19 +545,119 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>2184.371330084281</v>
+        <v>507.2009852429924</v>
       </c>
       <c r="D6" t="n">
         <v>1500</v>
       </c>
       <c r="E6" t="n">
-        <v>450.6451297740327</v>
+        <v>466.9654057349896</v>
       </c>
       <c r="F6" t="n">
-        <v>857.3955073347217</v>
+        <v>886.1562661123647</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>64</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2135.527146272234</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1500</v>
+      </c>
+      <c r="E7" t="n">
+        <v>527.5487730867658</v>
+      </c>
+      <c r="F7" t="n">
+        <v>950.8942286852177</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>547.8085094871341</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1500</v>
+      </c>
+      <c r="E8" t="n">
+        <v>500.9139139457083</v>
+      </c>
+      <c r="F8" t="n">
+        <v>935.4559132762812</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>557.6323942244364</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1500</v>
+      </c>
+      <c r="E9" t="n">
+        <v>511.2995171506442</v>
+      </c>
+      <c r="F9" t="n">
+        <v>897.3191306581153</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>491.9717572709463</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1500</v>
+      </c>
+      <c r="E10" t="n">
+        <v>469.7719128676806</v>
+      </c>
+      <c r="F10" t="n">
+        <v>867.534308455666</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="n">
+        <v>498.5914671003533</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="E11" t="n">
+        <v>429.929044104556</v>
+      </c>
+      <c r="F11" t="n">
+        <v>847.4310521269317</v>
       </c>
     </row>
   </sheetData>

</xml_diff>